<commit_message>
hotfix in view list users, update name download files, change label, change word english to spanish
</commit_message>
<xml_diff>
--- a/teg_asovac_src/static_env/media_root/cargamasiva/Arbitros.xlsx
+++ b/teg_asovac_src/static_env/media_root/cargamasiva/Arbitros.xlsx
@@ -31,19 +31,19 @@
     <t xml:space="preserve">Nombre de usuario (*)</t>
   </si>
   <si>
-    <t xml:space="preserve">Correo electronico (*)</t>
+    <t xml:space="preserve">Correo electrónico (*)</t>
   </si>
   <si>
     <t xml:space="preserve">Área (*)</t>
   </si>
   <si>
-    <t xml:space="preserve">Subarea 1 (*)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subarea 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subarea 3</t>
+    <t xml:space="preserve">Subárea 1 (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subárea 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subárea 3</t>
   </si>
   <si>
     <t xml:space="preserve">Género (*)</t>
@@ -235,8 +235,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
update value for field genero and change name area,subarea by code
</commit_message>
<xml_diff>
--- a/teg_asovac_src/static_env/media_root/cargamasiva/Arbitros.xlsx
+++ b/teg_asovac_src/static_env/media_root/cargamasiva/Arbitros.xlsx
@@ -85,13 +85,13 @@
     <t xml:space="preserve">paredesp@yopmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Biociencias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parasitología</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bioquímica</t>
+    <t xml:space="preserve">BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQM</t>
   </si>
   <si>
     <t xml:space="preserve">Masculino</t>
@@ -235,8 +235,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>